<commit_message>
- add a method to the worksheet that will print a single based on a well id, prod date, and product. Was mostly a hack...
</commit_message>
<xml_diff>
--- a/excel-app/database/database.xlsx
+++ b/excel-app/database/database.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\git\python-playground\excel-app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\git\python-playground\excel-app\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Roy Module Construct" sheetId="1" r:id="rId1"/>
@@ -18,20 +18,21 @@
     <sheet name="RoyaltyMaster" sheetId="2" r:id="rId4"/>
     <sheet name="Lease" sheetId="4" r:id="rId5"/>
     <sheet name="Well" sheetId="9" r:id="rId6"/>
-    <sheet name="MonthlyLots" sheetId="5" r:id="rId7"/>
-    <sheet name="Monthly" sheetId="13" r:id="rId8"/>
-    <sheet name="Calc" sheetId="14" r:id="rId9"/>
-    <sheet name="ProducingEntity" sheetId="11" r:id="rId10"/>
-    <sheet name="ExternalValues" sheetId="6" r:id="rId11"/>
-    <sheet name="ProductClauses" sheetId="7" r:id="rId12"/>
-    <sheet name="ECONData" sheetId="10" r:id="rId13"/>
+    <sheet name="Monthly" sheetId="5" r:id="rId7"/>
+    <sheet name=" Monthly 1" sheetId="13" r:id="rId8"/>
+    <sheet name="Calc" sheetId="15" r:id="rId9"/>
+    <sheet name="Calc 1" sheetId="14" r:id="rId10"/>
+    <sheet name="ProducingEntity" sheetId="11" r:id="rId11"/>
+    <sheet name="ExternalValues" sheetId="6" r:id="rId12"/>
+    <sheet name="ProductClauses" sheetId="7" r:id="rId13"/>
+    <sheet name="ECONData" sheetId="10" r:id="rId14"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="216">
   <si>
     <t>Lease Type</t>
   </si>
@@ -658,6 +659,27 @@
   </si>
   <si>
     <t>GorrMessage</t>
+  </si>
+  <si>
+    <t>dprod = 0.135135 = 100 / 740 is between 0.0 - 250.0 for a RR of 2.0%</t>
+  </si>
+  <si>
+    <t>mprod = 100 is between 0.0 - 250.0 for a RR of 2.0%</t>
+  </si>
+  <si>
+    <t>MOP &lt; 25 - RR = 0.</t>
+  </si>
+  <si>
+    <t>fixed for a RR of 2.0%</t>
+  </si>
+  <si>
+    <t>dprod = 2.083333 = 100 / 48 is between 0.0 - 250.0 for a RR of 2.0%</t>
+  </si>
+  <si>
+    <t>dprod = 0.208333 = 10 / 48 is between 0.0 - 250.0 for a RR of 2.0%</t>
+  </si>
+  <si>
+    <t>dprod = 4.166667 = 200 / 48 is between 0.0 - 250.0 for a RR of 2.0%</t>
   </si>
 </sst>
 </file>
@@ -1862,6 +1884,101 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z1"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H1" t="s">
+        <v>190</v>
+      </c>
+      <c r="I1" t="s">
+        <v>191</v>
+      </c>
+      <c r="J1" t="s">
+        <v>192</v>
+      </c>
+      <c r="K1" t="s">
+        <v>193</v>
+      </c>
+      <c r="L1" t="s">
+        <v>194</v>
+      </c>
+      <c r="M1" t="s">
+        <v>195</v>
+      </c>
+      <c r="N1" t="s">
+        <v>196</v>
+      </c>
+      <c r="O1" t="s">
+        <v>197</v>
+      </c>
+      <c r="P1" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>199</v>
+      </c>
+      <c r="R1" t="s">
+        <v>200</v>
+      </c>
+      <c r="S1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T1" t="s">
+        <v>202</v>
+      </c>
+      <c r="U1" t="s">
+        <v>203</v>
+      </c>
+      <c r="V1" t="s">
+        <v>204</v>
+      </c>
+      <c r="W1" t="s">
+        <v>205</v>
+      </c>
+      <c r="X1" t="s">
+        <v>206</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>207</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1900,7 +2017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -1926,7 +2043,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -1977,7 +2094,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE48"/>
   <sheetViews>
@@ -6968,7 +7085,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8303,7 +8420,7 @@
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -10039,9 +10156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:I28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10131,13 +10246,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -10219,6 +10332,2223 @@
         <v>208</v>
       </c>
     </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>201501</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H2">
+        <v>14</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>12</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>2680.44</v>
+      </c>
+      <c r="R2">
+        <v>446.74073199999998</v>
+      </c>
+      <c r="S2">
+        <v>3127.1807319999998</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>3127.1807319999998</v>
+      </c>
+      <c r="X2">
+        <v>0.08</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>201501</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H3">
+        <v>14</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>12</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>2680.44</v>
+      </c>
+      <c r="R3">
+        <v>446.74073199999998</v>
+      </c>
+      <c r="S3">
+        <v>3127.1807319999998</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>3127.1807319999998</v>
+      </c>
+      <c r="X3">
+        <v>0.08</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>201501</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H4">
+        <v>14</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>12</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>2680.44</v>
+      </c>
+      <c r="R4">
+        <v>446.74073199999998</v>
+      </c>
+      <c r="S4">
+        <v>3127.1807319999998</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>3127.1807319999998</v>
+      </c>
+      <c r="X4">
+        <v>0.08</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>201501</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>27.11</v>
+      </c>
+      <c r="D5">
+        <v>626</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>221.123456</v>
+      </c>
+      <c r="H5">
+        <v>15.5</v>
+      </c>
+      <c r="I5">
+        <v>20.85</v>
+      </c>
+      <c r="J5">
+        <v>50</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>15</v>
+      </c>
+      <c r="N5">
+        <v>0.5</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>3316.85</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>110.561728</v>
+      </c>
+      <c r="S5">
+        <v>3427.411728</v>
+      </c>
+      <c r="T5">
+        <v>32.913552499999987</v>
+      </c>
+      <c r="U5">
+        <v>1.9135525</v>
+      </c>
+      <c r="V5">
+        <v>34.827105000000003</v>
+      </c>
+      <c r="W5">
+        <v>3392.5846230000002</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>201501</v>
+      </c>
+      <c r="B6">
+        <v>2000</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>221.123456</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>201501</v>
+      </c>
+      <c r="B7">
+        <v>2000</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>9.3399999999999997E-2</v>
+      </c>
+      <c r="F7">
+        <v>2.34</v>
+      </c>
+      <c r="G7">
+        <v>221.123456</v>
+      </c>
+      <c r="H7">
+        <v>1.75</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>7</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>1.75</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>386.97</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>386.97</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>386.97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>201501</v>
+      </c>
+      <c r="B8">
+        <v>2000</v>
+      </c>
+      <c r="C8">
+        <v>23.12</v>
+      </c>
+      <c r="D8">
+        <v>1734</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>221.123456</v>
+      </c>
+      <c r="H8">
+        <v>7.2249999999999996</v>
+      </c>
+      <c r="I8">
+        <v>14.45</v>
+      </c>
+      <c r="J8">
+        <v>14.45</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>7.2249999999999996</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>1597.62</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>1597.62</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>1597.62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>201501</v>
+      </c>
+      <c r="B9">
+        <v>2001</v>
+      </c>
+      <c r="C9">
+        <v>27.11</v>
+      </c>
+      <c r="D9">
+        <v>626</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>221.123456</v>
+      </c>
+      <c r="H9">
+        <v>5.2125000000000004</v>
+      </c>
+      <c r="I9">
+        <v>20.85</v>
+      </c>
+      <c r="J9">
+        <v>20.85</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>5.2125000000000004</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>1152.6099999999999</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>1152.6099999999999</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>1152.6099999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>201501</v>
+      </c>
+      <c r="B10">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>9.3399999999999997E-2</v>
+      </c>
+      <c r="F10">
+        <v>2.34</v>
+      </c>
+      <c r="G10">
+        <v>221.123456</v>
+      </c>
+      <c r="H10">
+        <v>1.75</v>
+      </c>
+      <c r="I10">
+        <v>7</v>
+      </c>
+      <c r="J10">
+        <v>7</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>1.75</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>386.97</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>386.97</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>386.97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>201502</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>34.9</v>
+      </c>
+      <c r="D11">
+        <v>805</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H11">
+        <v>29.95825</v>
+      </c>
+      <c r="I11">
+        <v>26.85</v>
+      </c>
+      <c r="J11">
+        <v>26.85</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <v>28.058250000000001</v>
+      </c>
+      <c r="N11">
+        <v>1.9</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>6267.38</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>424.4036954</v>
+      </c>
+      <c r="S11">
+        <v>6691.7836954000004</v>
+      </c>
+      <c r="T11">
+        <v>63.614995753750001</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>63.614995753750001</v>
+      </c>
+      <c r="W11">
+        <v>6628.1686996462504</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>201503</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0.1237</v>
+      </c>
+      <c r="F12">
+        <v>3.09</v>
+      </c>
+      <c r="G12">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H12">
+        <v>10.352</v>
+      </c>
+      <c r="I12">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="J12">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <v>8.3520000000000003</v>
+      </c>
+      <c r="N12">
+        <v>2</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1865.59</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>446.74073199999998</v>
+      </c>
+      <c r="S12">
+        <v>2312.3307319999999</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>1.2780061599999999</v>
+      </c>
+      <c r="V12">
+        <v>1.2780061599999999</v>
+      </c>
+      <c r="W12">
+        <v>2311.0527258400002</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>201504</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>53.69</v>
+      </c>
+      <c r="D13">
+        <v>1239</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H13">
+        <v>51.625</v>
+      </c>
+      <c r="I13">
+        <v>41.3</v>
+      </c>
+      <c r="J13">
+        <v>41.3</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>51.625</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>11531.5</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>11531.5</v>
+      </c>
+      <c r="T13">
+        <v>109.62336437499999</v>
+      </c>
+      <c r="U13">
+        <v>6.3733643750000004</v>
+      </c>
+      <c r="V13">
+        <v>115.99672875</v>
+      </c>
+      <c r="W13">
+        <v>11415.50327125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>201504</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>53.69</v>
+      </c>
+      <c r="D14">
+        <v>1239</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H14">
+        <v>51.625</v>
+      </c>
+      <c r="I14">
+        <v>41.3</v>
+      </c>
+      <c r="J14">
+        <v>41.3</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>51.625</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>11531.5</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>11531.5</v>
+      </c>
+      <c r="T14">
+        <v>109.62336437499999</v>
+      </c>
+      <c r="U14">
+        <v>6.3733643750000004</v>
+      </c>
+      <c r="V14">
+        <v>115.99672875</v>
+      </c>
+      <c r="W14">
+        <v>11415.50327125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>201504</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>28.6</v>
+      </c>
+      <c r="D15">
+        <v>660</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>221.123456</v>
+      </c>
+      <c r="H15">
+        <v>15.5</v>
+      </c>
+      <c r="I15">
+        <v>22</v>
+      </c>
+      <c r="J15">
+        <v>50</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>15</v>
+      </c>
+      <c r="N15">
+        <v>0.5</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>3316.85</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>110.561728</v>
+      </c>
+      <c r="S15">
+        <v>3427.411728</v>
+      </c>
+      <c r="T15">
+        <v>32.913552499999987</v>
+      </c>
+      <c r="U15">
+        <v>1.9135525</v>
+      </c>
+      <c r="V15">
+        <v>34.827105000000003</v>
+      </c>
+      <c r="W15">
+        <v>3392.5846230000002</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>201503</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>34.340000000000003</v>
+      </c>
+      <c r="D16">
+        <v>793</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H16">
+        <v>29.498449999999998</v>
+      </c>
+      <c r="I16">
+        <v>26.41</v>
+      </c>
+      <c r="J16">
+        <v>26.41</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>27.59845</v>
+      </c>
+      <c r="N16">
+        <v>1.9</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>6164.68</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>424.4036954</v>
+      </c>
+      <c r="S16">
+        <v>6589.0836954000006</v>
+      </c>
+      <c r="T16">
+        <v>62.638631144750001</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>62.638631144750001</v>
+      </c>
+      <c r="W16">
+        <v>6526.4450642552501</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>201503</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H17">
+        <v>1.2</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0.2</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>223.37</v>
+      </c>
+      <c r="R17">
+        <v>44.674073200000009</v>
+      </c>
+      <c r="S17">
+        <v>268.04407320000001</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>268.04407320000001</v>
+      </c>
+      <c r="X17">
+        <v>0.25</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>201503</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H18">
+        <v>14</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <v>12</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>2680.44</v>
+      </c>
+      <c r="R18">
+        <v>446.74073199999998</v>
+      </c>
+      <c r="S18">
+        <v>3127.1807319999998</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>3127.1807319999998</v>
+      </c>
+      <c r="X18">
+        <v>0.25</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>201503</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H19">
+        <v>14</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="O19">
+        <v>12</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>2680.44</v>
+      </c>
+      <c r="R19">
+        <v>446.74073199999998</v>
+      </c>
+      <c r="S19">
+        <v>3127.1807319999998</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>3127.1807319999998</v>
+      </c>
+      <c r="X19">
+        <v>0.25</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>201503</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H20">
+        <v>14</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>2</v>
+      </c>
+      <c r="O20">
+        <v>12</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>2680.44</v>
+      </c>
+      <c r="R20">
+        <v>446.74073199999998</v>
+      </c>
+      <c r="S20">
+        <v>3127.1807319999998</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>3127.1807319999998</v>
+      </c>
+      <c r="X20">
+        <v>0.25</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>201504</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H21">
+        <v>38.4</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>2</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>4</v>
+      </c>
+      <c r="O21">
+        <v>34.4</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>7683.94</v>
+      </c>
+      <c r="R21">
+        <v>893.48146400000007</v>
+      </c>
+      <c r="S21">
+        <v>8577.4214639999991</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>8577.4214639999991</v>
+      </c>
+      <c r="X21">
+        <v>0.33</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>201504</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H22">
+        <v>38.4</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>4</v>
+      </c>
+      <c r="O22">
+        <v>34.4</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>7683.94</v>
+      </c>
+      <c r="R22">
+        <v>893.48146400000007</v>
+      </c>
+      <c r="S22">
+        <v>8577.4214639999991</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>8577.4214639999991</v>
+      </c>
+      <c r="X22">
+        <v>0.33</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>201504</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H23">
+        <v>38.4</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>4</v>
+      </c>
+      <c r="O23">
+        <v>34.4</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>7683.94</v>
+      </c>
+      <c r="R23">
+        <v>893.48146400000007</v>
+      </c>
+      <c r="S23">
+        <v>8577.4214639999991</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>8577.4214639999991</v>
+      </c>
+      <c r="X23">
+        <v>0.33</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>201504</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>24.7</v>
+      </c>
+      <c r="D24">
+        <v>570</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H24">
+        <v>16.149999999999999</v>
+      </c>
+      <c r="I24">
+        <v>19</v>
+      </c>
+      <c r="J24">
+        <v>19</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>16.149999999999999</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>3607.43</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>3607.43</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>3607.43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>201504</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>24.7</v>
+      </c>
+      <c r="D25">
+        <v>570</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H25">
+        <v>16.149999999999999</v>
+      </c>
+      <c r="I25">
+        <v>19</v>
+      </c>
+      <c r="J25">
+        <v>19</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>16.149999999999999</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>3607.43</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>3607.43</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>3607.43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>201504</v>
+      </c>
+      <c r="B26">
+        <v>11</v>
+      </c>
+      <c r="C26">
+        <v>35.65</v>
+      </c>
+      <c r="D26">
+        <v>823</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>221.123456</v>
+      </c>
+      <c r="H26">
+        <v>62</v>
+      </c>
+      <c r="I26">
+        <v>27.42</v>
+      </c>
+      <c r="J26">
+        <v>50</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>2</v>
+      </c>
+      <c r="M26">
+        <v>60</v>
+      </c>
+      <c r="N26">
+        <v>2</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>13267.41</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>442.24691200000001</v>
+      </c>
+      <c r="S26">
+        <v>13709.656912</v>
+      </c>
+      <c r="T26">
+        <v>131.65421000000001</v>
+      </c>
+      <c r="U26">
+        <v>7.65421</v>
+      </c>
+      <c r="V26">
+        <v>139.30842000000001</v>
+      </c>
+      <c r="W26">
+        <v>13570.348491999999</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>201504</v>
+      </c>
+      <c r="B27">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>37.81</v>
+      </c>
+      <c r="D27">
+        <v>873</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H27">
+        <v>33.988000000000007</v>
+      </c>
+      <c r="I27">
+        <v>29.08</v>
+      </c>
+      <c r="J27">
+        <v>29.08</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>2</v>
+      </c>
+      <c r="M27">
+        <v>31.98800000000001</v>
+      </c>
+      <c r="N27">
+        <v>2</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>7145.17</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>446.74073199999998</v>
+      </c>
+      <c r="S27">
+        <v>7591.9107320000003</v>
+      </c>
+      <c r="T27">
+        <v>72.171988540000015</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>72.171988540000015</v>
+      </c>
+      <c r="W27">
+        <v>7519.7387434599996</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>201504</v>
+      </c>
+      <c r="B28">
+        <v>14</v>
+      </c>
+      <c r="C28">
+        <v>28.6</v>
+      </c>
+      <c r="D28">
+        <v>660</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H28">
+        <v>27.5</v>
+      </c>
+      <c r="I28">
+        <v>22</v>
+      </c>
+      <c r="J28">
+        <v>22</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>27.5</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>6142.69</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>6142.69</v>
+      </c>
+      <c r="T28">
+        <v>58.395012500000007</v>
+      </c>
+      <c r="U28">
+        <v>3.3950125</v>
+      </c>
+      <c r="V28">
+        <v>61.790025000000007</v>
+      </c>
+      <c r="W28">
+        <v>6080.8999749999994</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>201504</v>
+      </c>
+      <c r="B29">
+        <v>15</v>
+      </c>
+      <c r="C29">
+        <v>40.58</v>
+      </c>
+      <c r="D29">
+        <v>937</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H29">
+        <v>26.528500000000001</v>
+      </c>
+      <c r="I29">
+        <v>31.21</v>
+      </c>
+      <c r="J29">
+        <v>31.21</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>26.528500000000001</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>5925.68</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <v>5925.68</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>5925.68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>201504</v>
+      </c>
+      <c r="B30">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <v>41.65</v>
+      </c>
+      <c r="D30">
+        <v>961</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>221.123456</v>
+      </c>
+      <c r="H30">
+        <v>62</v>
+      </c>
+      <c r="I30">
+        <v>32.04</v>
+      </c>
+      <c r="J30">
+        <v>50</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>2</v>
+      </c>
+      <c r="M30">
+        <v>60</v>
+      </c>
+      <c r="N30">
+        <v>2</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>13267.41</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>442.24691200000001</v>
+      </c>
+      <c r="S30">
+        <v>13709.656912</v>
+      </c>
+      <c r="T30">
+        <v>131.65421000000001</v>
+      </c>
+      <c r="U30">
+        <v>7.65421</v>
+      </c>
+      <c r="V30">
+        <v>139.30842000000001</v>
+      </c>
+      <c r="W30">
+        <v>13570.348491999999</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>201504</v>
+      </c>
+      <c r="B31">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <v>53.69</v>
+      </c>
+      <c r="D31">
+        <v>1239</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>223.37036599999999</v>
+      </c>
+      <c r="H31">
+        <v>35.104999999999997</v>
+      </c>
+      <c r="I31">
+        <v>41.3</v>
+      </c>
+      <c r="J31">
+        <v>41.3</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>35.104999999999997</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>7841.42</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>7841.42</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>7841.42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- start hacking at the sqlite load code from excel. It kinda works
</commit_message>
<xml_diff>
--- a/excel-app/database/database.xlsx
+++ b/excel-app/database/database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Roy Module Construct" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="213">
   <si>
     <t>Lease Type</t>
   </si>
@@ -527,15 +527,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>(Used for Examples</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Sask Oil SKProvCrownVar / SaskWellHead / No Deductions / Fourth Tier </t>
-  </si>
-  <si>
-    <t>(Used for testing well update</t>
   </si>
   <si>
     <t>(Used to test Royalty Maser Tests</t>
@@ -1792,7 +1783,7 @@
         <v>42307</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E28" s="23">
         <v>3559.12</v>
@@ -1801,7 +1792,7 @@
         <v>2909.71</v>
       </c>
       <c r="G28" s="22" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H28" s="20"/>
     </row>
@@ -1811,7 +1802,7 @@
         <v>42307</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E29" s="23">
         <v>12092.5</v>
@@ -1820,7 +1811,7 @@
         <v>11281.02</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H29" s="25"/>
     </row>
@@ -1830,7 +1821,7 @@
         <v>42282</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E30" s="23">
         <v>4000</v>
@@ -1839,7 +1830,7 @@
         <v>2795.11</v>
       </c>
       <c r="G30" s="22" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H30" s="25"/>
     </row>
@@ -1849,7 +1840,7 @@
         <v>42282</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E31" s="28">
         <v>164</v>
@@ -1858,7 +1849,7 @@
         <v>114.6</v>
       </c>
       <c r="G31" s="26" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H31" s="30"/>
     </row>
@@ -1900,76 +1891,76 @@
         <v>75</v>
       </c>
       <c r="C1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" t="s">
         <v>185</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>186</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>187</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>188</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>189</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>190</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>191</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>192</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>193</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>194</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>195</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>196</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>197</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>199</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>200</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>201</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>202</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>203</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>204</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>205</v>
-      </c>
-      <c r="X1" t="s">
-        <v>206</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>207</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -6750,24 +6741,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -6800,7 +6791,7 @@
         <v>52</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C1" t="s">
         <v>63</v>
@@ -6824,7 +6815,7 @@
         <v>134</v>
       </c>
       <c r="J1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K1" t="s">
         <v>164</v>
@@ -6841,7 +6832,7 @@
         <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E2">
         <v>1.2</v>
@@ -6859,7 +6850,7 @@
         <v>133</v>
       </c>
       <c r="J2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -6873,7 +6864,7 @@
         <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E3">
         <v>1.1000000000000001</v>
@@ -6888,7 +6879,7 @@
         <v>133</v>
       </c>
       <c r="J3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -6902,7 +6893,7 @@
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E4">
         <v>0.9</v>
@@ -6914,7 +6905,7 @@
         <v>133</v>
       </c>
       <c r="J4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -6974,7 +6965,7 @@
         <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -6983,7 +6974,7 @@
         <v>157</v>
       </c>
       <c r="J7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -6997,7 +6988,7 @@
         <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -7006,7 +6997,7 @@
         <v>157</v>
       </c>
       <c r="J8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -7020,7 +7011,7 @@
         <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -7029,7 +7020,7 @@
         <v>157</v>
       </c>
       <c r="J9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -7072,7 +7063,7 @@
         <v>154</v>
       </c>
       <c r="K11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -7101,7 +7092,7 @@
         <v>52</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C1" t="s">
         <v>49</v>
@@ -7286,7 +7277,7 @@
         <v>2345</v>
       </c>
       <c r="F11" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -7296,11 +7287,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7315,7 +7306,7 @@
     <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -7332,7 +7323,7 @@
         <v>52</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G1" t="s">
         <v>149</v>
@@ -7352,11 +7343,8 @@
       <c r="L1" t="s">
         <v>163</v>
       </c>
-      <c r="M1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7387,14 +7375,14 @@
       <c r="J2" s="17">
         <v>0.25</v>
       </c>
-      <c r="K2">
-        <v>1</v>
+      <c r="K2" s="18">
+        <v>41974</v>
       </c>
       <c r="L2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7425,14 +7413,14 @@
       <c r="J3" s="17">
         <v>0.95</v>
       </c>
-      <c r="K3">
-        <v>1</v>
+      <c r="K3" s="18">
+        <v>41974</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7464,7 +7452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7496,7 +7484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7525,7 +7513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7560,7 +7548,7 @@
         <v>41974</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7595,7 +7583,7 @@
         <v>41974</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7630,7 +7618,7 @@
         <v>41974</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -7662,7 +7650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -7694,7 +7682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -7726,7 +7714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -7758,7 +7746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -7790,7 +7778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -7822,7 +7810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -7854,7 +7842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -7886,7 +7874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -7918,7 +7906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -7950,7 +7938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -7982,7 +7970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -8014,7 +8002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -8046,7 +8034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -8078,7 +8066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -8110,7 +8098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -8142,7 +8130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -8174,7 +8162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>30</v>
       </c>
@@ -8206,7 +8194,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>31</v>
       </c>
@@ -8232,7 +8220,7 @@
         <v>40513</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>32</v>
       </c>
@@ -8258,7 +8246,7 @@
         <v>40513</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>33</v>
       </c>
@@ -8284,7 +8272,7 @@
         <v>41974</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1000</v>
       </c>
@@ -8309,11 +8297,8 @@
       <c r="K31" s="18">
         <v>41609</v>
       </c>
-      <c r="M31" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2000</v>
       </c>
@@ -8344,11 +8329,8 @@
       <c r="J32" s="17">
         <v>0.25</v>
       </c>
-      <c r="M32" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2001</v>
       </c>
@@ -8380,7 +8362,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3000</v>
       </c>
@@ -8404,9 +8386,6 @@
       </c>
       <c r="K34" s="18">
         <v>40513</v>
-      </c>
-      <c r="M34" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -8457,7 +8436,7 @@
         <v>142</v>
       </c>
       <c r="G1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H1" t="s">
         <v>55</v>
@@ -10183,7 +10162,7 @@
         <v>142</v>
       </c>
       <c r="G1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H1" t="s">
         <v>55</v>
@@ -10248,7 +10227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -10260,76 +10239,76 @@
         <v>75</v>
       </c>
       <c r="C1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" t="s">
         <v>185</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>186</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>187</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>188</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>189</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>190</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>191</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>192</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>193</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>194</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>195</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>196</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>197</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>199</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>200</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>201</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>202</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>203</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>204</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>205</v>
-      </c>
-      <c r="X1" t="s">
-        <v>206</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>207</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -10406,7 +10385,7 @@
         <v>0.08</v>
       </c>
       <c r="Z2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -10483,7 +10462,7 @@
         <v>0.08</v>
       </c>
       <c r="Z3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -10560,7 +10539,7 @@
         <v>0.08</v>
       </c>
       <c r="Z4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -10634,7 +10613,7 @@
         <v>3392.5846230000002</v>
       </c>
       <c r="Z5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -10708,7 +10687,7 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -11066,7 +11045,7 @@
         <v>6628.1686996462504</v>
       </c>
       <c r="Z11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
@@ -11140,7 +11119,7 @@
         <v>2311.0527258400002</v>
       </c>
       <c r="Z12" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
@@ -11356,7 +11335,7 @@
         <v>3392.5846230000002</v>
       </c>
       <c r="Z15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -11430,7 +11409,7 @@
         <v>6526.4450642552501</v>
       </c>
       <c r="Z16" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
@@ -11507,7 +11486,7 @@
         <v>0.25</v>
       </c>
       <c r="Z17" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
@@ -11584,7 +11563,7 @@
         <v>0.25</v>
       </c>
       <c r="Z18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
@@ -11661,7 +11640,7 @@
         <v>0.25</v>
       </c>
       <c r="Z19" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
@@ -11738,7 +11717,7 @@
         <v>0.25</v>
       </c>
       <c r="Z20" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
@@ -11815,7 +11794,7 @@
         <v>0.33</v>
       </c>
       <c r="Z21" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
@@ -11892,7 +11871,7 @@
         <v>0.33</v>
       </c>
       <c r="Z22" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -11969,7 +11948,7 @@
         <v>0.33</v>
       </c>
       <c r="Z23" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -12185,7 +12164,7 @@
         <v>13570.348491999999</v>
       </c>
       <c r="Z26" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -12259,7 +12238,7 @@
         <v>7519.7387434599996</v>
       </c>
       <c r="Z27" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -12475,7 +12454,7 @@
         <v>13570.348491999999</v>
       </c>
       <c r="Z30" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>